<commit_message>
Update format of BRPSPTY
</commit_message>
<xml_diff>
--- a/InputData/elec/BRPSPTY/BAU RPS Percentage This Year.xlsx
+++ b/InputData/elec/BRPSPTY/BAU RPS Percentage This Year.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\elec\BRPSPTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-eu\InputData\elec\BRPSPTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620F8629-D6B3-480E-A714-94960ADDEB92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3934D029-18E0-4706-AC34-19574D5E7356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39555" yWindow="4515" windowWidth="20100" windowHeight="16125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="jrc potencia scenario" sheetId="16" r:id="rId2"/>
     <sheet name="BRPSPTY" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
   <si>
     <t>BRPSPTY BAU Renewable Portfolio Std Percentage This Year</t>
   </si>
   <si>
-    <t>Year</t>
-  </si>
-  <si>
     <t>Note:</t>
   </si>
   <si>
@@ -56,9 +53,6 @@
     <t>Sources:</t>
   </si>
   <si>
-    <t>RPS Fraction (dimensionless)</t>
-  </si>
-  <si>
     <t>https://ec.europa.eu/jrc/en/publication/eur-scientific-and-technical-research-reports/potencia-central-scenario-eu-energy-outlook-2050</t>
   </si>
   <si>
@@ -84,6 +78,258 @@
   </si>
   <si>
     <t>The scenario reflects existing policies and measures that were in place by the end of 2017.</t>
+  </si>
+  <si>
+    <t>Note that this variable is populating the Future Year subscript.  It is not a normal time-series data variable.  Therefore, this sheet must include a value for every year that exists in the Future Year subscript (and no other years should be present).</t>
+  </si>
+  <si>
+    <t>Unit: dimensionless</t>
+  </si>
+  <si>
+    <t>RPS Fraction</t>
+  </si>
+  <si>
+    <t>Year2020</t>
+  </si>
+  <si>
+    <t>Year2021</t>
+  </si>
+  <si>
+    <t>Year2022</t>
+  </si>
+  <si>
+    <t>Year2023</t>
+  </si>
+  <si>
+    <t>Year2024</t>
+  </si>
+  <si>
+    <t>Year2025</t>
+  </si>
+  <si>
+    <t>Year2026</t>
+  </si>
+  <si>
+    <t>Year2027</t>
+  </si>
+  <si>
+    <t>Year2028</t>
+  </si>
+  <si>
+    <t>Year2029</t>
+  </si>
+  <si>
+    <t>Year2030</t>
+  </si>
+  <si>
+    <t>Year2031</t>
+  </si>
+  <si>
+    <t>Year2032</t>
+  </si>
+  <si>
+    <t>Year2033</t>
+  </si>
+  <si>
+    <t>Year2034</t>
+  </si>
+  <si>
+    <t>Year2035</t>
+  </si>
+  <si>
+    <t>Year2036</t>
+  </si>
+  <si>
+    <t>Year2037</t>
+  </si>
+  <si>
+    <t>Year2038</t>
+  </si>
+  <si>
+    <t>Year2039</t>
+  </si>
+  <si>
+    <t>Year2040</t>
+  </si>
+  <si>
+    <t>Year2041</t>
+  </si>
+  <si>
+    <t>Year2042</t>
+  </si>
+  <si>
+    <t>Year2043</t>
+  </si>
+  <si>
+    <t>Year2044</t>
+  </si>
+  <si>
+    <t>Year2045</t>
+  </si>
+  <si>
+    <t>Year2046</t>
+  </si>
+  <si>
+    <t>Year2047</t>
+  </si>
+  <si>
+    <t>Year2048</t>
+  </si>
+  <si>
+    <t>Year2049</t>
+  </si>
+  <si>
+    <t>Year2050</t>
+  </si>
+  <si>
+    <t>Year2051</t>
+  </si>
+  <si>
+    <t>Year2052</t>
+  </si>
+  <si>
+    <t>Year2053</t>
+  </si>
+  <si>
+    <t>Year2054</t>
+  </si>
+  <si>
+    <t>Year2055</t>
+  </si>
+  <si>
+    <t>Year2056</t>
+  </si>
+  <si>
+    <t>Year2057</t>
+  </si>
+  <si>
+    <t>Year2058</t>
+  </si>
+  <si>
+    <t>Year2059</t>
+  </si>
+  <si>
+    <t>Year2060</t>
+  </si>
+  <si>
+    <t>Year2061</t>
+  </si>
+  <si>
+    <t>Year2062</t>
+  </si>
+  <si>
+    <t>Year2063</t>
+  </si>
+  <si>
+    <t>Year2064</t>
+  </si>
+  <si>
+    <t>Year2065</t>
+  </si>
+  <si>
+    <t>Year2066</t>
+  </si>
+  <si>
+    <t>Year2067</t>
+  </si>
+  <si>
+    <t>Year2068</t>
+  </si>
+  <si>
+    <t>Year2069</t>
+  </si>
+  <si>
+    <t>Year2070</t>
+  </si>
+  <si>
+    <t>Year2071</t>
+  </si>
+  <si>
+    <t>Year2072</t>
+  </si>
+  <si>
+    <t>Year2073</t>
+  </si>
+  <si>
+    <t>Year2074</t>
+  </si>
+  <si>
+    <t>Year2075</t>
+  </si>
+  <si>
+    <t>Year2076</t>
+  </si>
+  <si>
+    <t>Year2077</t>
+  </si>
+  <si>
+    <t>Year2078</t>
+  </si>
+  <si>
+    <t>Year2079</t>
+  </si>
+  <si>
+    <t>Year2080</t>
+  </si>
+  <si>
+    <t>Year2081</t>
+  </si>
+  <si>
+    <t>Year2082</t>
+  </si>
+  <si>
+    <t>Year2083</t>
+  </si>
+  <si>
+    <t>Year2084</t>
+  </si>
+  <si>
+    <t>Year2085</t>
+  </si>
+  <si>
+    <t>Year2086</t>
+  </si>
+  <si>
+    <t>Year2087</t>
+  </si>
+  <si>
+    <t>Year2088</t>
+  </si>
+  <si>
+    <t>Year2089</t>
+  </si>
+  <si>
+    <t>Year2090</t>
+  </si>
+  <si>
+    <t>Year2091</t>
+  </si>
+  <si>
+    <t>Year2092</t>
+  </si>
+  <si>
+    <t>Year2093</t>
+  </si>
+  <si>
+    <t>Year2094</t>
+  </si>
+  <si>
+    <t>Year2095</t>
+  </si>
+  <si>
+    <t>Year2096</t>
+  </si>
+  <si>
+    <t>Year2097</t>
+  </si>
+  <si>
+    <t>Year2098</t>
+  </si>
+  <si>
+    <t>Year2099</t>
+  </si>
+  <si>
+    <t>Year2100</t>
   </si>
 </sst>
 </file>
@@ -94,7 +340,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00%;\-0.00%;&quot;&quot;"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,6 +535,14 @@
     <font>
       <b/>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -720,7 +974,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -747,6 +1001,10 @@
     </xf>
     <xf numFmtId="1" fontId="26" fillId="33" borderId="14" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
@@ -1143,82 +1401,82 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="122.73046875" customWidth="1"/>
+    <col min="2" max="2" width="122.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B4" s="7" t="s">
-        <v>8</v>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B5" s="3" t="s">
-        <v>14</v>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B6" s="3" t="s">
-        <v>9</v>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B7" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B7" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1236,11 +1494,11 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="12">
         <v>2000</v>
@@ -1396,9 +1654,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:52" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:52" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="9">
         <v>0</v>
@@ -1564,261 +1822,547 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:CD4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="BE1" workbookViewId="0">
+      <selection activeCell="AG2" sqref="AG2:CD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>2017</v>
-      </c>
-      <c r="C1">
-        <v>2018</v>
-      </c>
-      <c r="D1">
-        <v>2019</v>
-      </c>
-      <c r="E1">
-        <v>2020</v>
-      </c>
-      <c r="F1">
-        <v>2021</v>
-      </c>
-      <c r="G1">
-        <v>2022</v>
-      </c>
-      <c r="H1">
-        <v>2023</v>
-      </c>
-      <c r="I1">
-        <v>2024</v>
-      </c>
-      <c r="J1">
-        <v>2025</v>
-      </c>
-      <c r="K1">
-        <v>2026</v>
-      </c>
-      <c r="L1">
-        <v>2027</v>
-      </c>
-      <c r="M1">
-        <v>2028</v>
-      </c>
-      <c r="N1">
-        <v>2029</v>
-      </c>
-      <c r="O1">
-        <v>2030</v>
-      </c>
-      <c r="P1">
-        <v>2031</v>
-      </c>
-      <c r="Q1">
-        <v>2032</v>
-      </c>
-      <c r="R1">
-        <v>2033</v>
-      </c>
-      <c r="S1">
-        <v>2034</v>
-      </c>
-      <c r="T1">
-        <v>2035</v>
-      </c>
-      <c r="U1">
-        <v>2036</v>
-      </c>
-      <c r="V1">
-        <v>2037</v>
-      </c>
-      <c r="W1">
-        <v>2038</v>
-      </c>
-      <c r="X1">
-        <v>2039</v>
-      </c>
-      <c r="Y1">
-        <v>2040</v>
-      </c>
-      <c r="Z1">
-        <v>2041</v>
-      </c>
-      <c r="AA1">
-        <v>2042</v>
-      </c>
-      <c r="AB1">
-        <v>2043</v>
-      </c>
-      <c r="AC1">
-        <v>2044</v>
-      </c>
-      <c r="AD1">
-        <v>2045</v>
-      </c>
-      <c r="AE1">
-        <v>2046</v>
-      </c>
-      <c r="AF1">
-        <v>2047</v>
-      </c>
-      <c r="AG1">
-        <v>2048</v>
-      </c>
-      <c r="AH1">
-        <v>2049</v>
-      </c>
-      <c r="AI1">
-        <v>2050</v>
+    <row r="1" spans="1:82" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="S1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="T1" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="V1" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y1" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z1" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA1" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB1" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC1" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD1" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE1" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF1" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG1" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH1" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI1" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ1" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL1" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM1" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN1" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO1" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP1" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR1" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="AT1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU1" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV1" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="AW1" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="AX1" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="AY1" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ1" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="BA1" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="BB1" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="BC1" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="BD1" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="BE1" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="BF1" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="BG1" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BH1" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BI1" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="BJ1" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="BK1" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="BL1" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="BM1" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="BN1" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="BO1" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="BP1" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="BQ1" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="BR1" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="BS1" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="BT1" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="BU1" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="BV1" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="BW1" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="BX1" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="BY1" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="BZ1" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="CA1" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="CB1" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="CC1" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="CD1" s="14" t="s">
+        <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B2" s="6">
-        <f>'jrc potencia scenario'!S2</f>
-        <v>0.31157935861539099</v>
-      </c>
-      <c r="C2" s="6">
-        <f>'jrc potencia scenario'!T2</f>
-        <v>0.3306420781129758</v>
-      </c>
-      <c r="D2" s="6">
-        <f>'jrc potencia scenario'!U2</f>
-        <v>0.35173630230492003</v>
-      </c>
-      <c r="E2" s="6">
         <f>'jrc potencia scenario'!V2</f>
         <v>0.37362225683235017</v>
       </c>
-      <c r="F2" s="6">
+      <c r="C2" s="6">
         <f>'jrc potencia scenario'!W2</f>
         <v>0.3841225186336788</v>
       </c>
-      <c r="G2" s="6">
+      <c r="D2" s="6">
         <f>'jrc potencia scenario'!X2</f>
         <v>0.3903708710536114</v>
       </c>
-      <c r="H2" s="6">
+      <c r="E2" s="6">
         <f>'jrc potencia scenario'!Y2</f>
         <v>0.40013620296428692</v>
       </c>
-      <c r="I2" s="6">
+      <c r="F2" s="6">
         <f>'jrc potencia scenario'!Z2</f>
         <v>0.41258327127583361</v>
       </c>
-      <c r="J2" s="6">
+      <c r="G2" s="6">
         <f>'jrc potencia scenario'!AA2</f>
         <v>0.42300962122915753</v>
       </c>
-      <c r="K2" s="6">
+      <c r="H2" s="6">
         <f>'jrc potencia scenario'!AB2</f>
         <v>0.43494444652722247</v>
       </c>
-      <c r="L2" s="6">
+      <c r="I2" s="6">
         <f>'jrc potencia scenario'!AC2</f>
         <v>0.44634726546652925</v>
       </c>
-      <c r="M2" s="6">
+      <c r="J2" s="6">
         <f>'jrc potencia scenario'!AD2</f>
         <v>0.45468776112649734</v>
       </c>
-      <c r="N2" s="6">
+      <c r="K2" s="6">
         <f>'jrc potencia scenario'!AE2</f>
         <v>0.46660874524999185</v>
       </c>
-      <c r="O2" s="6">
+      <c r="L2" s="6">
         <f>'jrc potencia scenario'!AF2</f>
         <v>0.48142956448987939</v>
       </c>
-      <c r="P2" s="6">
+      <c r="M2" s="6">
         <f>'jrc potencia scenario'!AG2</f>
         <v>0.49497982569518406</v>
       </c>
-      <c r="Q2" s="6">
+      <c r="N2" s="6">
         <f>'jrc potencia scenario'!AH2</f>
         <v>0.50844330419859818</v>
       </c>
-      <c r="R2" s="6">
+      <c r="O2" s="6">
         <f>'jrc potencia scenario'!AI2</f>
         <v>0.52565844986650323</v>
       </c>
-      <c r="S2" s="6">
+      <c r="P2" s="6">
         <f>'jrc potencia scenario'!AJ2</f>
         <v>0.54404351088112624</v>
       </c>
-      <c r="T2" s="6">
+      <c r="Q2" s="6">
         <f>'jrc potencia scenario'!AK2</f>
         <v>0.56407268915699038</v>
       </c>
-      <c r="U2" s="6">
+      <c r="R2" s="6">
         <f>'jrc potencia scenario'!AL2</f>
         <v>0.58593893616468806</v>
       </c>
-      <c r="V2" s="6">
+      <c r="S2" s="6">
         <f>'jrc potencia scenario'!AM2</f>
         <v>0.60788955860572536</v>
       </c>
-      <c r="W2" s="6">
+      <c r="T2" s="6">
         <f>'jrc potencia scenario'!AN2</f>
         <v>0.62669487816737035</v>
       </c>
-      <c r="X2" s="6">
+      <c r="U2" s="6">
         <f>'jrc potencia scenario'!AO2</f>
         <v>0.64074676826603705</v>
       </c>
-      <c r="Y2" s="6">
+      <c r="V2" s="6">
         <f>'jrc potencia scenario'!AP2</f>
         <v>0.65324194366038479</v>
       </c>
-      <c r="Z2" s="6">
+      <c r="W2" s="6">
         <f>'jrc potencia scenario'!AQ2</f>
         <v>0.66720923308981062</v>
       </c>
-      <c r="AA2" s="6">
+      <c r="X2" s="6">
         <f>'jrc potencia scenario'!AR2</f>
         <v>0.67501331784370533</v>
       </c>
-      <c r="AB2" s="6">
+      <c r="Y2" s="6">
         <f>'jrc potencia scenario'!AS2</f>
         <v>0.68743104195281413</v>
       </c>
-      <c r="AC2" s="6">
+      <c r="Z2" s="6">
         <f>'jrc potencia scenario'!AT2</f>
         <v>0.69364367384730152</v>
       </c>
-      <c r="AD2" s="6">
+      <c r="AA2" s="6">
         <f>'jrc potencia scenario'!AU2</f>
         <v>0.70455518241672821</v>
       </c>
-      <c r="AE2" s="6">
+      <c r="AB2" s="6">
         <f>'jrc potencia scenario'!AV2</f>
         <v>0.71049507913572596</v>
       </c>
-      <c r="AF2" s="6">
+      <c r="AC2" s="6">
         <f>'jrc potencia scenario'!AW2</f>
         <v>0.71526254976367276</v>
       </c>
-      <c r="AG2" s="6">
+      <c r="AD2" s="6">
         <f>'jrc potencia scenario'!AX2</f>
         <v>0.72015149651598476</v>
       </c>
-      <c r="AH2" s="6">
+      <c r="AE2" s="6">
         <f>'jrc potencia scenario'!AY2</f>
         <v>0.72424401737320443</v>
       </c>
-      <c r="AI2" s="6">
+      <c r="AF2" s="6">
         <f>'jrc potencia scenario'!AZ2</f>
         <v>0.73037831195435232</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+      <c r="AT2">
+        <v>0</v>
+      </c>
+      <c r="AU2">
+        <v>0</v>
+      </c>
+      <c r="AV2">
+        <v>0</v>
+      </c>
+      <c r="AW2">
+        <v>0</v>
+      </c>
+      <c r="AX2">
+        <v>0</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+      <c r="AZ2">
+        <v>0</v>
+      </c>
+      <c r="BA2">
+        <v>0</v>
+      </c>
+      <c r="BB2">
+        <v>0</v>
+      </c>
+      <c r="BC2">
+        <v>0</v>
+      </c>
+      <c r="BD2">
+        <v>0</v>
+      </c>
+      <c r="BE2">
+        <v>0</v>
+      </c>
+      <c r="BF2">
+        <v>0</v>
+      </c>
+      <c r="BG2">
+        <v>0</v>
+      </c>
+      <c r="BH2">
+        <v>0</v>
+      </c>
+      <c r="BI2">
+        <v>0</v>
+      </c>
+      <c r="BJ2">
+        <v>0</v>
+      </c>
+      <c r="BK2">
+        <v>0</v>
+      </c>
+      <c r="BL2">
+        <v>0</v>
+      </c>
+      <c r="BM2">
+        <v>0</v>
+      </c>
+      <c r="BN2">
+        <v>0</v>
+      </c>
+      <c r="BO2">
+        <v>0</v>
+      </c>
+      <c r="BP2">
+        <v>0</v>
+      </c>
+      <c r="BQ2">
+        <v>0</v>
+      </c>
+      <c r="BR2">
+        <v>0</v>
+      </c>
+      <c r="BS2">
+        <v>0</v>
+      </c>
+      <c r="BT2">
+        <v>0</v>
+      </c>
+      <c r="BU2">
+        <v>0</v>
+      </c>
+      <c r="BV2">
+        <v>0</v>
+      </c>
+      <c r="BW2">
+        <v>0</v>
+      </c>
+      <c r="BX2">
+        <v>0</v>
+      </c>
+      <c r="BY2">
+        <v>0</v>
+      </c>
+      <c r="BZ2">
+        <v>0</v>
+      </c>
+      <c r="CA2">
+        <v>0</v>
+      </c>
+      <c r="CB2">
+        <v>0</v>
+      </c>
+      <c r="CC2">
+        <v>0</v>
+      </c>
+      <c r="CD2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:82" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FoPITY and BVS updates
</commit_message>
<xml_diff>
--- a/InputData/elec/BRPSPTY/BAU RPS Percentage This Year.xlsx
+++ b/InputData/elec/BRPSPTY/BAU RPS Percentage This Year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Francis Swint\Vensim\eps-eu\InputData\elec\BRPSPTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\Vensim files from GitHub\EPS EU\InputData\elec\BRPSPTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294DB4DF-C685-4E79-BE9E-BB08B4DF9FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138CD4E2-9B22-43E1-AF50-7DA6A6CB7E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5780" yWindow="2240" windowWidth="14400" windowHeight="8170" firstSheet="2" activeTab="5" xr2:uid="{8223E8A3-2731-4425-BB39-7296F4257534}"/>
+    <workbookView xWindow="615" yWindow="2280" windowWidth="22755" windowHeight="13815" firstSheet="2" activeTab="5" xr2:uid="{8223E8A3-2731-4425-BB39-7296F4257534}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="8" r:id="rId1"/>
@@ -6330,22 +6330,22 @@
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.81640625" style="79"/>
-    <col min="3" max="3" width="45.26953125" style="79" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.81640625" style="79"/>
+    <col min="1" max="2" width="10.85546875" style="79"/>
+    <col min="3" max="3" width="45.28515625" style="79" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.85546875" style="79"/>
   </cols>
   <sheetData>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="80" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="81"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="81" t="s">
         <v>1</v>
       </c>
@@ -6356,7 +6356,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="81"/>
       <c r="C14" s="81" t="s">
         <v>4</v>
@@ -6365,7 +6365,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="81"/>
       <c r="C15" s="81" t="s">
         <v>6</v>
@@ -6374,7 +6374,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="81"/>
       <c r="C16" s="81" t="s">
         <v>6</v>
@@ -6383,90 +6383,90 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="81"/>
       <c r="C17" s="82"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="81" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="104" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="83"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="104" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="83"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="104" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="83"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="104"/>
       <c r="C23" s="83"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="104" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="83"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="104" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="83"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="104" t="s">
         <v>15</v>
       </c>
       <c r="C26" s="83"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="104"/>
       <c r="C27" s="83"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="104" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="83"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="104" t="s">
         <v>17</v>
       </c>
       <c r="C29" s="83"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="99" t="s">
         <v>18</v>
       </c>
       <c r="C30" s="83"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="146" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="83"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="146" t="s">
         <v>20</v>
       </c>
       <c r="C32" s="83"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="83"/>
       <c r="C33" s="83"/>
     </row>
@@ -6490,19 +6490,19 @@
       <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="96.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="96.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="108" t="s">
         <v>21</v>
       </c>
@@ -6529,7 +6529,7 @@
       <c r="U1" s="109"/>
       <c r="V1" s="118"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="113" t="s">
         <v>23</v>
       </c>
@@ -6540,7 +6540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>24</v>
       </c>
@@ -6605,7 +6605,7 @@
       <c r="AA3" s="40"/>
       <c r="AB3" s="40"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>26</v>
       </c>
@@ -6667,7 +6667,7 @@
       <c r="AA4" s="40"/>
       <c r="AB4" s="40"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>29</v>
       </c>
@@ -6729,7 +6729,7 @@
       <c r="AA5" s="42"/>
       <c r="AB5" s="42"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>32</v>
       </c>
@@ -6791,7 +6791,7 @@
       <c r="AA6" s="42"/>
       <c r="AB6" s="42"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>35</v>
       </c>
@@ -6848,7 +6848,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>38</v>
       </c>
@@ -6902,7 +6902,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="105">
         <v>2021</v>
@@ -6919,7 +6919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>41</v>
       </c>
@@ -6936,7 +6936,7 @@
       <c r="V10" s="12"/>
       <c r="X10" s="71"/>
     </row>
-    <row r="11" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>43</v>
       </c>
@@ -6951,7 +6951,7 @@
       <c r="V11" s="12"/>
       <c r="X11" s="71"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>44</v>
       </c>
@@ -6990,7 +6990,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="L13" s="12"/>
       <c r="N13" s="25" t="s">
@@ -7029,7 +7029,7 @@
         <v>849.1525652317888</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -7071,7 +7071,7 @@
         <v>275.41521509782802</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="113" t="s">
         <v>47</v>
       </c>
@@ -7115,7 +7115,7 @@
         <v>810.26050207252831</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>45</v>
       </c>
@@ -7161,7 +7161,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>46</v>
       </c>
@@ -7201,7 +7201,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>35</v>
       </c>
@@ -7241,7 +7241,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>38</v>
       </c>
@@ -7289,7 +7289,7 @@
         <v>2337.8282824021453</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>41</v>
       </c>
@@ -7335,7 +7335,7 @@
         <v>3600.9504270677526</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>43</v>
       </c>
@@ -7356,7 +7356,7 @@
       <c r="U21" s="60"/>
       <c r="V21" s="60"/>
     </row>
-    <row r="22" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>44</v>
       </c>
@@ -7368,7 +7368,7 @@
       </c>
       <c r="L22" s="12"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>48</v>
       </c>
@@ -7391,7 +7391,7 @@
       <c r="U23" s="118"/>
       <c r="V23" s="138"/>
     </row>
-    <row r="24" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>49</v>
       </c>
@@ -7406,7 +7406,7 @@
       <c r="O24" s="42"/>
       <c r="U24" s="12"/>
     </row>
-    <row r="25" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="L25" s="12"/>
       <c r="N25" s="130" t="s">
@@ -7415,7 +7415,7 @@
       <c r="O25" s="40"/>
       <c r="U25" s="12"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>51</v>
       </c>
@@ -7472,7 +7472,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>32</v>
       </c>
@@ -7518,7 +7518,7 @@
       </c>
       <c r="U27" s="12"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>35</v>
       </c>
@@ -7564,7 +7564,7 @@
       </c>
       <c r="U28" s="12"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>38</v>
       </c>
@@ -7637,7 +7637,7 @@
         <v>513894.97433035483</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>41</v>
       </c>
@@ -7704,7 +7704,7 @@
         <v>95023.201612612349</v>
       </c>
     </row>
-    <row r="31" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>43</v>
       </c>
@@ -7771,7 +7771,7 @@
         <v>412615.47339026764</v>
       </c>
     </row>
-    <row r="32" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>44</v>
       </c>
@@ -7809,7 +7809,7 @@
       <c r="N32" s="11"/>
       <c r="U32" s="12"/>
     </row>
-    <row r="33" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
       <c r="L33" s="12"/>
       <c r="N33" s="130" t="s">
@@ -7818,7 +7818,7 @@
       <c r="O33" s="40"/>
       <c r="U33" s="12"/>
     </row>
-    <row r="34" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="115" t="s">
         <v>54</v>
       </c>
@@ -7858,7 +7858,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="35" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="11"/>
       <c r="L35" s="12"/>
       <c r="N35" s="11" t="s">
@@ -7866,7 +7866,7 @@
       </c>
       <c r="U35" s="12"/>
     </row>
-    <row r="36" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="141" t="s">
         <v>55</v>
       </c>
@@ -7908,7 +7908,7 @@
       </c>
       <c r="U36" s="12"/>
     </row>
-    <row r="37" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="147" t="s">
         <v>56</v>
       </c>
@@ -7984,7 +7984,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="139" t="s">
         <v>7</v>
       </c>
@@ -8048,7 +8048,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="139" t="s">
         <v>53</v>
       </c>
@@ -8106,7 +8106,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="140" t="s">
         <v>47</v>
       </c>
@@ -8147,7 +8147,7 @@
       <c r="U40" s="72"/>
       <c r="V40" s="72"/>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>58</v>
       </c>
@@ -8181,21 +8181,21 @@
       <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.1796875" customWidth="1"/>
-    <col min="13" max="14" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="37.81640625" customWidth="1"/>
-    <col min="17" max="18" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="24" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="13" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="37.85546875" customWidth="1"/>
+    <col min="17" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="24" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>59</v>
       </c>
@@ -8206,7 +8206,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>62</v>
       </c>
@@ -8238,7 +8238,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="24">
         <v>2012</v>
@@ -8307,7 +8307,7 @@
         <v>710642</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>63</v>
       </c>
@@ -8374,7 +8374,7 @@
         <v>2321</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>64</v>
       </c>
@@ -8449,7 +8449,7 @@
         <v>712963</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>65</v>
       </c>
@@ -8522,7 +8522,7 @@
         <v>85545</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K7" s="1"/>
       <c r="L7" s="18"/>
       <c r="M7" s="18"/>
@@ -8561,7 +8561,7 @@
         <v>396365</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="K8" s="1"/>
       <c r="L8" s="18"/>
       <c r="M8" s="18"/>
@@ -8590,7 +8590,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -8631,7 +8631,7 @@
         <v>91485</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="P10" s="11" t="s">
         <v>35</v>
       </c>
@@ -8660,7 +8660,7 @@
         <v>12285</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P11" s="7" t="s">
         <v>38</v>
       </c>
@@ -8691,7 +8691,7 @@
         <v>37320</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
@@ -8711,7 +8711,7 @@
       <c r="W12" s="4"/>
       <c r="X12" s="4"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>67</v>
       </c>
@@ -8760,7 +8760,7 @@
       <c r="W13" s="60"/>
       <c r="X13" s="60"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>26</v>
       </c>
@@ -8814,7 +8814,7 @@
       <c r="W14" s="60"/>
       <c r="X14" s="60"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>64</v>
       </c>
@@ -8868,7 +8868,7 @@
       <c r="W15" s="60"/>
       <c r="X15" s="60"/>
     </row>
-    <row r="16" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -8923,7 +8923,7 @@
       <c r="W16" s="60"/>
       <c r="X16" s="60"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="J17" s="78" t="s">
         <v>69</v>
       </c>
@@ -8937,7 +8937,7 @@
       <c r="W17" s="60"/>
       <c r="X17" s="60"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="P18" s="4"/>
@@ -8950,7 +8950,7 @@
       <c r="W18" s="60"/>
       <c r="X18" s="60"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="71"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
@@ -8959,7 +8959,7 @@
       <c r="F19" s="18"/>
       <c r="P19" s="4"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="18"/>
@@ -8967,28 +8967,28 @@
       <c r="F20" s="18"/>
       <c r="P20" s="4"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="18"/>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="71"/>
       <c r="P26" s="84"/>
       <c r="Q26" s="84"/>
@@ -8998,7 +8998,7 @@
       <c r="U26" s="84"/>
       <c r="V26" s="84"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="71"/>
       <c r="P27" s="84"/>
       <c r="Q27" s="85"/>
@@ -9008,7 +9008,7 @@
       <c r="U27" s="85"/>
       <c r="V27" s="85"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="P28" s="84"/>
       <c r="Q28" s="85"/>
       <c r="R28" s="85"/>
@@ -9017,7 +9017,7 @@
       <c r="U28" s="85"/>
       <c r="V28" s="85"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="P29" s="84"/>
       <c r="Q29" s="85"/>
       <c r="R29" s="85"/>
@@ -9026,7 +9026,7 @@
       <c r="U29" s="85"/>
       <c r="V29" s="85"/>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="P30" s="84"/>
       <c r="Q30" s="85"/>
       <c r="R30" s="85"/>
@@ -9035,7 +9035,7 @@
       <c r="U30" s="85"/>
       <c r="V30" s="85"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="P31" s="84"/>
       <c r="Q31" s="85"/>
       <c r="R31" s="85"/>
@@ -9044,7 +9044,7 @@
       <c r="U31" s="85"/>
       <c r="V31" s="85"/>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="P32" s="84"/>
       <c r="Q32" s="85"/>
       <c r="R32" s="85"/>
@@ -9053,7 +9053,7 @@
       <c r="U32" s="85"/>
       <c r="V32" s="85"/>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="P33" s="84"/>
       <c r="Q33" s="85"/>
       <c r="R33" s="85"/>
@@ -9062,7 +9062,7 @@
       <c r="U33" s="85"/>
       <c r="V33" s="85"/>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -9075,7 +9075,7 @@
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="F35" s="27"/>
       <c r="G35" s="27"/>
@@ -9084,7 +9084,7 @@
       <c r="J35" s="27"/>
       <c r="K35" s="27"/>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="F36" s="27"/>
       <c r="G36" s="27"/>
@@ -9093,7 +9093,7 @@
       <c r="J36" s="27"/>
       <c r="K36" s="27"/>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="F37" s="27"/>
       <c r="G37" s="27"/>
@@ -9102,7 +9102,7 @@
       <c r="J37" s="27"/>
       <c r="K37" s="27"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="F38" s="27"/>
       <c r="G38" s="27"/>
@@ -9111,7 +9111,7 @@
       <c r="J38" s="27"/>
       <c r="K38" s="27"/>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="F39" s="27"/>
       <c r="G39" s="27"/>
@@ -9120,7 +9120,7 @@
       <c r="J39" s="27"/>
       <c r="K39" s="27"/>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -9145,12 +9145,12 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29"/>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -9160,7 +9160,7 @@
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
       <c r="B2" s="31">
         <v>2020</v>
@@ -9184,7 +9184,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>70</v>
       </c>
@@ -9196,7 +9196,7 @@
       <c r="G3" s="34"/>
       <c r="H3" s="35"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
         <v>71</v>
       </c>
@@ -9222,7 +9222,7 @@
         <v>3420676.8662906797</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>72</v>
       </c>
@@ -9252,7 +9252,7 @@
         <v>3.0285886950903902E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
         <v>73</v>
       </c>
@@ -9278,7 +9278,7 @@
         <v>2542270.2940083593</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="s">
         <v>74</v>
       </c>
@@ -9304,7 +9304,7 @@
         <v>207321.14157649977</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="44" t="s">
         <v>75</v>
       </c>
@@ -9330,7 +9330,7 @@
         <v>368186.56193746976</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="45" t="s">
         <v>76</v>
       </c>
@@ -9356,7 +9356,7 @@
         <v>190933.72364244243</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="45" t="s">
         <v>77</v>
       </c>
@@ -9382,7 +9382,7 @@
         <v>177252.83829502721</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
         <v>78</v>
       </c>
@@ -9408,7 +9408,7 @@
         <v>1350438.0753462599</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
         <v>65</v>
       </c>
@@ -9434,7 +9434,7 @@
         <v>990669.90900849062</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="45" t="s">
         <v>64</v>
       </c>
@@ -9460,7 +9460,7 @@
         <v>359768.16633776913</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
         <v>79</v>
       </c>
@@ -9486,7 +9486,7 @@
         <v>599657.36191915383</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
         <v>80</v>
       </c>
@@ -9512,7 +9512,7 @@
         <v>16667.153228975938</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="46"/>
       <c r="B16" s="40"/>
       <c r="C16" s="40"/>
@@ -9522,7 +9522,7 @@
       <c r="G16" s="40"/>
       <c r="H16" s="41"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="46"/>
       <c r="B17" s="40"/>
       <c r="C17" s="40"/>
@@ -9532,7 +9532,7 @@
       <c r="G17" s="40"/>
       <c r="H17" s="41"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
         <v>81</v>
       </c>
@@ -9558,7 +9558,7 @@
         <v>1386347.2096200143</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="39" t="s">
         <v>73</v>
       </c>
@@ -9584,7 +9584,7 @@
         <v>1213108.7488916744</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="44" t="s">
         <v>74</v>
       </c>
@@ -9610,7 +9610,7 @@
         <v>55588.655806831353</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="44" t="s">
         <v>82</v>
       </c>
@@ -9636,7 +9636,7 @@
         <v>133135.17602102979</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="45" t="s">
         <v>76</v>
       </c>
@@ -9662,7 +9662,7 @@
         <v>89864.065417295002</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="45" t="s">
         <v>77</v>
       </c>
@@ -9688,7 +9688,7 @@
         <v>43271.110603734829</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="44" t="s">
         <v>78</v>
       </c>
@@ -9714,7 +9714,7 @@
         <v>507638.67500287993</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="45" t="s">
         <v>65</v>
       </c>
@@ -9740,7 +9740,7 @@
         <v>412615.47339026764</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="45" t="s">
         <v>64</v>
       </c>
@@ -9766,7 +9766,7 @@
         <v>95023.201612612349</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="44" t="s">
         <v>79</v>
       </c>
@@ -9792,7 +9792,7 @@
         <v>513894.97433035483</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="47" t="s">
         <v>83</v>
       </c>
@@ -9818,8 +9818,8 @@
         <v>2851.2677305788761</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>51</v>
       </c>
@@ -9845,7 +9845,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="45" t="s">
         <v>65</v>
       </c>
@@ -9878,7 +9878,7 @@
         <v>2.4009519101855803</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="45" t="s">
         <v>64</v>
       </c>
@@ -9911,7 +9911,7 @@
         <v>3.7861086580145011</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="47" t="s">
         <v>79</v>
       </c>
@@ -9944,7 +9944,7 @@
         <v>1.1668869941772715</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>84</v>
       </c>
@@ -9970,7 +9970,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -10016,12 +10016,12 @@
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="29"/>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -10030,7 +10030,7 @@
       <c r="F1" s="29"/>
       <c r="G1" s="29"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="68"/>
       <c r="B2" s="65">
         <v>2005</v>
@@ -10051,7 +10051,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="64" t="s">
         <v>70</v>
       </c>
@@ -10062,7 +10062,7 @@
       <c r="F3" s="34"/>
       <c r="G3" s="34"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="67" t="s">
         <v>71</v>
       </c>
@@ -10085,7 +10085,7 @@
         <v>3153537.5898405975</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="63" t="s">
         <v>85</v>
       </c>
@@ -10108,7 +10108,7 @@
         <v>515398.0748518536</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="63" t="s">
         <v>73</v>
       </c>
@@ -10131,7 +10131,7 @@
         <v>2050530.87578808</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="56" t="s">
         <v>74</v>
       </c>
@@ -10154,7 +10154,7 @@
         <v>167171.97368861208</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="56" t="s">
         <v>75</v>
       </c>
@@ -10177,7 +10177,7 @@
         <v>361836.01941072679</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="57" t="s">
         <v>76</v>
       </c>
@@ -10200,7 +10200,7 @@
         <v>190294.89092214324</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="57" t="s">
         <v>77</v>
       </c>
@@ -10223,7 +10223,7 @@
         <v>171541.12848858361</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="56" t="s">
         <v>78</v>
       </c>
@@ -10246,7 +10246,7 @@
         <v>1078584.1832632506</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="57" t="s">
         <v>65</v>
       </c>
@@ -10269,7 +10269,7 @@
         <v>830898.54292468261</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="57" t="s">
         <v>64</v>
       </c>
@@ -10292,7 +10292,7 @@
         <v>247685.64033856773</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="56" t="s">
         <v>79</v>
       </c>
@@ -10315,7 +10315,7 @@
         <v>435636.65246775595</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="56" t="s">
         <v>80</v>
       </c>
@@ -10338,7 +10338,7 @@
         <v>7302.0469577341519</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="63" t="s">
         <v>86</v>
       </c>
@@ -10361,7 +10361,7 @@
         <v>587608.63920066366</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="56" t="s">
         <v>87</v>
       </c>
@@ -10384,7 +10384,7 @@
         <v>138743.08584963548</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="56" t="s">
         <v>88</v>
       </c>
@@ -10407,7 +10407,7 @@
         <v>8045.2816189790883</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="56" t="s">
         <v>89</v>
       </c>
@@ -10430,7 +10430,7 @@
         <v>440820.27173204912</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="63" t="s">
         <v>90</v>
       </c>
@@ -10453,7 +10453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="66"/>
       <c r="B21" s="40"/>
       <c r="C21" s="40"/>
@@ -10462,7 +10462,7 @@
       <c r="F21" s="40"/>
       <c r="G21" s="40"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="67" t="s">
         <v>81</v>
       </c>
@@ -10485,7 +10485,7 @@
         <v>1336372.912873992</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="63" t="s">
         <v>85</v>
       </c>
@@ -10508,7 +10508,7 @@
         <v>93931.180000000008</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="63" t="s">
         <v>73</v>
       </c>
@@ -10531,7 +10531,7 @@
         <v>1006740.4357627709</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="56" t="s">
         <v>74</v>
       </c>
@@ -10554,7 +10554,7 @@
         <v>63738.931428774791</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="56" t="s">
         <v>82</v>
       </c>
@@ -10577,7 +10577,7 @@
         <v>131477.14878095107</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="57" t="s">
         <v>76</v>
       </c>
@@ -10600,7 +10600,7 @@
         <v>89534.913947263471</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="57" t="s">
         <v>77</v>
       </c>
@@ -10623,7 +10623,7 @@
         <v>41942.234833687638</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="56" t="s">
         <v>78</v>
       </c>
@@ -10646,7 +10646,7 @@
         <v>427346.16747689148</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="57" t="s">
         <v>65</v>
       </c>
@@ -10669,7 +10669,7 @@
         <v>360987.9386301139</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="57" t="s">
         <v>64</v>
       </c>
@@ -10692,7 +10692,7 @@
         <v>66358.228846777594</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="56" t="s">
         <v>79</v>
       </c>
@@ -10715,7 +10715,7 @@
         <v>383044.78807615401</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="56" t="s">
         <v>83</v>
       </c>
@@ -10738,7 +10738,7 @@
         <v>1133.4000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="63" t="s">
         <v>86</v>
       </c>
@@ -10761,7 +10761,7 @@
         <v>235701.29711122054</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="56" t="s">
         <v>87</v>
       </c>
@@ -10784,7 +10784,7 @@
         <v>63432.780613092924</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="56" t="s">
         <v>88</v>
       </c>
@@ -10807,7 +10807,7 @@
         <v>13513.310953866192</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="56" t="s">
         <v>89</v>
       </c>
@@ -10830,7 +10830,7 @@
         <v>158755.20554426141</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="63" t="s">
         <v>90</v>
       </c>
@@ -10865,17 +10865,18 @@
   </sheetPr>
   <dimension ref="A1:CD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BJ1" workbookViewId="0">
-      <selection activeCell="BN6" sqref="BN6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="32" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="32" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A1" s="71" t="s">
         <v>91</v>
       </c>
@@ -11123,7 +11124,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="2" spans="1:82" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>92</v>
       </c>

</xml_diff>